<commit_message>
Changes in Potential AE form #97
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/potential_ae.xlsx
+++ b/zazic-scale-up/forms/app/potential_ae.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-81\itech-aurum\forms\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-97\zazic-scale-up\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D06A958-FDBA-4325-A085-B392E3C05E41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB552D5-9E2B-46EB-8C25-785247CB365E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -278,9 +278,6 @@
     <t>Why was client NOT asked to seek care?</t>
   </si>
   <si>
-    <t>selected(${client_return}, 'no')</t>
-  </si>
-  <si>
     <t>list_name</t>
   </si>
   <si>
@@ -417,6 +414,9 @@
   </si>
   <si>
     <t>Study Nurse will use this form to record every potential AE reported, even if multiple per client, including: 1) A client sends a YES SMS to note a potential AE; 2) A client sends a question about a symptom via SMS; and 3) A client requests a follow-up call.</t>
+  </si>
+  <si>
+    <t>selected(${client_return}, 'no') and selected(${ae}, 'yes')</t>
   </si>
 </sst>
 </file>
@@ -1009,10 +1009,10 @@
   <dimension ref="A1:AMJ30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
@@ -1069,7 +1069,7 @@
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:27">
@@ -1384,7 +1384,7 @@
       <c r="Z13" s="7"/>
       <c r="AA13" s="7"/>
     </row>
-    <row r="14" spans="1:27" ht="86.25">
+    <row r="14" spans="1:27">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>44</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>129</v>
+        <v>46</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
@@ -1405,7 +1405,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" ht="86.25">
       <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>46</v>
+        <v>128</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8" t="s">
@@ -1770,7 +1770,7 @@
         <v>82</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>83</v>
+        <v>129</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
@@ -1811,7 +1811,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
@@ -1822,7 +1822,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>1</v>
@@ -1839,7 +1839,7 @@
         <v>33</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1850,7 +1850,7 @@
         <v>52</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1858,10 +1858,10 @@
         <v>68</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="18" t="s">
         <v>87</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1874,10 +1874,10 @@
         <v>58</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>89</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1885,10 +1885,10 @@
         <v>58</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>91</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1896,10 +1896,10 @@
         <v>58</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="17" t="s">
         <v>93</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1907,10 +1907,10 @@
         <v>58</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>95</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1918,10 +1918,10 @@
         <v>58</v>
       </c>
       <c r="B10" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>97</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1929,10 +1929,10 @@
         <v>58</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>99</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1940,10 +1940,10 @@
         <v>58</v>
       </c>
       <c r="B12" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="17" t="s">
         <v>101</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1953,24 +1953,24 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>105</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2132,10 +2132,10 @@
         <v>48</v>
       </c>
       <c r="B31" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>101</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2143,7 +2143,7 @@
         <v>65</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>85</v>
@@ -2154,10 +2154,10 @@
         <v>65</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2165,10 +2165,10 @@
         <v>65</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2176,10 +2176,10 @@
         <v>74</v>
       </c>
       <c r="B37" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" t="s">
         <v>108</v>
-      </c>
-      <c r="C37" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2187,10 +2187,10 @@
         <v>74</v>
       </c>
       <c r="B38" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" t="s">
         <v>110</v>
-      </c>
-      <c r="C38" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2198,10 +2198,10 @@
         <v>74</v>
       </c>
       <c r="B39" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" t="s">
         <v>112</v>
-      </c>
-      <c r="C39" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2227,31 +2227,31 @@
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
       <c r="A1" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>118</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>119</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>120</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>121</v>
       </c>
       <c r="J1" s="19"/>
       <c r="K1" s="19"/>
@@ -2273,29 +2273,29 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>122</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>123</v>
       </c>
       <c r="C2" s="23">
         <v>43008</v>
       </c>
       <c r="D2" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>124</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>125</v>
       </c>
       <c r="F2" s="22"/>
       <c r="G2" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" s="22" t="s">
         <v>126</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>127</v>
       </c>
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>

</xml_diff>

<commit_message>
change to site nurse (#256)
* change to site nurse

* change in xls

Co-authored-by: Emmanuel Amodu <emmanuelamodu@Emmanuels-MacBook-Pro-2.local>
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/potential_ae.xlsx
+++ b/zazic-scale-up/forms/app/potential_ae.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-97\zazic-scale-up\forms\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmanuelamodu/Desktop/medic-mobile/config-itech/zazic-scale-up/forms/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB552D5-9E2B-46EB-8C25-785247CB365E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E92002-1855-9A42-847A-3AD4F317B5C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -413,10 +413,10 @@
     <t>instance::tag</t>
   </si>
   <si>
-    <t>Study Nurse will use this form to record every potential AE reported, even if multiple per client, including: 1) A client sends a YES SMS to note a potential AE; 2) A client sends a question about a symptom via SMS; and 3) A client requests a follow-up call.</t>
-  </si>
-  <si>
     <t>selected(${client_return}, 'no') and selected(${ae}, 'yes')</t>
+  </si>
+  <si>
+    <t>Site nurse will use this form to record every potential AE reported, even if multiple per client, including: 1) A client sends a YES SMS to note a potential AE; 2) A client sends a question about a symptom via SMS; and 3) A client requests a follow-up call.</t>
   </si>
 </sst>
 </file>
@@ -1009,25 +1009,25 @@
   <dimension ref="A1:AMJ30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="24.75" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="44.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.25" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" style="1"/>
-    <col min="7" max="7" width="19.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.5" style="1"/>
     <col min="9" max="9" width="34" style="1" customWidth="1"/>
     <col min="10" max="11" width="11.5" style="1"/>
-    <col min="12" max="12" width="20.25" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.1640625" style="1" customWidth="1"/>
     <col min="13" max="1024" width="11.5" style="1"/>
   </cols>
   <sheetData>
@@ -1166,7 +1166,7 @@
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
     </row>
-    <row r="6" spans="1:27" ht="43.5">
+    <row r="6" spans="1:27" ht="46">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1405,7 +1405,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:27" ht="86.25">
+    <row r="15" spans="1:27" ht="76">
       <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>45</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8" t="s">
@@ -1428,7 +1428,7 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
     </row>
-    <row r="16" spans="1:27" ht="29.25">
+    <row r="16" spans="1:27" ht="31">
       <c r="A16" s="8" t="s">
         <v>47</v>
       </c>
@@ -1520,7 +1520,7 @@
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
     </row>
-    <row r="20" spans="1:27" ht="29.25">
+    <row r="20" spans="1:27" ht="31">
       <c r="A20" s="8" t="s">
         <v>57</v>
       </c>
@@ -1629,7 +1629,7 @@
       <c r="Z22" s="7"/>
       <c r="AA22" s="7"/>
     </row>
-    <row r="23" spans="1:27" ht="29.25">
+    <row r="23" spans="1:27" ht="31">
       <c r="A23" s="8" t="s">
         <v>64</v>
       </c>
@@ -1770,7 +1770,7 @@
         <v>82</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="12"/>
@@ -1814,10 +1814,10 @@
       <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="17.875" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2216,13 +2216,13 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="43.75" customWidth="1"/>
-    <col min="3" max="3" width="32.875" customWidth="1"/>
-    <col min="4" max="4" width="20.875" customWidth="1"/>
-    <col min="16" max="26" width="8.875" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="16" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">

</xml_diff>